<commit_message>
creacion de pasajeros dinamicos y lector de URL para encontrar producto y total pasajeros datosFormularioJS-Promerica.py
</commit_message>
<xml_diff>
--- a/Ejercicios_Python/generarScriptJS/pasajeros.xlsx
+++ b/Ejercicios_Python/generarScriptJS/pasajeros.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poligran-my.sharepoint.com/personal/jeromero6_poligran_edu_co/Documents/EngSoftware/Python/Ejercicios_Python/generarScriptJS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_86257F671A0D27D480234FF725D472973CF4DD37" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5897B1DC-2E32-4F80-8A75-53EFCB0DAD19}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_40FD1F611A0D27D480234FF725D472978C7F84B5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4F3E72B-DD39-4F9E-A049-84BC36770ED6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,9 +383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>